<commit_message>
feat: refatoração e adição de funcionalidade de processamento de excel.
</commit_message>
<xml_diff>
--- a/example-export-template-excel/example.xlsx
+++ b/example-export-template-excel/example.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
     <t>Games</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -350,7 +350,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" sqref="B2:B100000" type="list">
+    <dataValidation allowBlank="true" sqref="D2:D100000" type="list">
       <formula1>"Super Mario,SONIC,Zelda,GTA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>